<commit_message>
Results of blanks in the subtitles document
Results of blanks in the subtitles document
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="119">
   <si>
     <t>Options</t>
   </si>
@@ -377,13 +377,42 @@
   </si>
   <si>
     <t>Subtitles of random sizes (max size = 20s)</t>
+  </si>
+  <si>
+    <t>Subtitles with blanks</t>
+  </si>
+  <si>
+    <t>dashed 10s segments
+Ts=Ts'=10s + blanks</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile full -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-blanks.mp4 -out manifest-test-dash-10s-blanks-full</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile simple -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-blanks.mp4 -out manifest-test-dash-10s-blanks-simple</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile main -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-blanks.mp4 -out manifest-test-dash-10s-blanks-main</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-blanks.mp4 -out manifest-test-dash-10s-blanks-onDemand</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile dashavc264:onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-blanks.mp4 -out manifest-test-dash-10s-blanks-dashavc264</t>
+  </si>
+  <si>
+    <t>Load, appear, can seek and see the subtitles, but does not play.
+THE SUBTITLE APPEARS TWICE BEFORE A BLANK !</t>
+  </si>
+  <si>
+    <t>Plays but THE SUBTITLE APPEARS TWICE BEFORE A BLANK !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,6 +476,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -623,7 +658,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="146">
+  <cellStyleXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -738,6 +773,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -843,7 +890,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="146">
+  <cellStyles count="158">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="113" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -916,6 +963,12 @@
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -987,6 +1040,12 @@
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="112" builtinId="21"/>
@@ -1318,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1886,7 +1945,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="120">
+    <row r="18" spans="1:11" ht="121" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>74</v>
       </c>
@@ -1921,9 +1980,67 @@
         <v>105</v>
       </c>
     </row>
+    <row r="19" spans="1:11" s="20" customFormat="1" ht="35" customHeight="1" thickBot="1">
+      <c r="A19" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" ht="105">
+      <c r="A20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="39" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="20" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="2" manualBreakCount="2">
+    <brk id="6" max="1048575" man="1"/>
+    <brk id="11" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Tests with subtitle document different from A/C content
Tests with subtitle document different from A/C content
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -2,13 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
-  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="AC = Subs" sheetId="1" r:id="rId1"/>
-    <sheet name="AC != Subs" sheetId="2" r:id="rId2"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="135">
   <si>
     <t>Options</t>
   </si>
@@ -406,13 +405,64 @@
   </si>
   <si>
     <t>Plays but THE SUBTITLE APPEARS TWICE BEFORE A BLANK !</t>
+  </si>
+  <si>
+    <t>Subtitles Shorter and Longer than A/C</t>
+  </si>
+  <si>
+    <t>dashed 10s segments
+Ts=Ts'=10s + A/C &gt;= subs</t>
+  </si>
+  <si>
+    <t>dashed 10s segments
+Ts=Ts'=10s + A/C &lt;= subs</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile full -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-shorter.mp4 -out manifest-test-dash-10s-shorter-full</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile simple -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-shorter.mp4 -out manifest-test-dash-10s-shorter-simple</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile main -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-shorter.mp4 -out manifest-test-dash-10s-shorter-main</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-shorter.mp4 -out manifest-test-dash-10s-shorter-onDemand</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile dashavc264:onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-shorter.mp4 -out manifest-test-dash-10s-shorter-dashavc264</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile full -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-longer.mp4 -out manifest-test-dash-10s-longer-full</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile simple -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-longer.mp4 -out manifest-test-dash-10s-longer-simple</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile main -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-longer.mp4 -out manifest-test-dash-10s-longer-main</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-longer.mp4 -out manifest-test-dash-10s-longer-onDemand</t>
+  </si>
+  <si>
+    <t>MP4Box -dash 10000 -profile dashavc264:onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-10s-longer.mp4 -out manifest-test-dash-10s-longer-dashavc264</t>
+  </si>
+  <si>
+    <t>Load, appear, can seek and see the subtitles, but does not play.
+VIDEO STOPS AT THE END OF SUBTITLE DOCUMENT.</t>
+  </si>
+  <si>
+    <t>Plays but VIDEO STOPS AT THE END OF SUBTITLE DOCUMENT.</t>
+  </si>
+  <si>
+    <t>All good (stops at the end of A/C)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,12 +530,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -526,7 +570,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -657,8 +701,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="158">
+  <cellStyleXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -817,8 +892,58 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -889,8 +1014,17 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="113" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="113" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="113" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="113" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="158">
+  <cellStyles count="208">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="113" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -969,6 +1103,31 @@
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1046,6 +1205,31 @@
     <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="112" builtinId="21"/>
@@ -1377,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1995,7 +2179,7 @@
       <c r="J19" s="22"/>
       <c r="K19" s="23"/>
     </row>
-    <row r="20" spans="1:11" ht="105">
+    <row r="20" spans="1:11" ht="106" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>111</v>
       </c>
@@ -2030,160 +2214,94 @@
         <v>116</v>
       </c>
     </row>
-  </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="39" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="20" max="16383" man="1"/>
-  </rowBreaks>
-  <colBreaks count="2" manualBreakCount="2">
-    <brk id="6" max="1048575" man="1"/>
-    <brk id="11" max="1048575" man="1"/>
-  </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="28.5" defaultRowHeight="43" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>10</v>
-      </c>
+    <row r="21" spans="1:11" s="20" customFormat="1" ht="35" customHeight="1">
+      <c r="A21" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
     </row>
-    <row r="2" spans="1:11" ht="43" customHeight="1" thickBot="1">
-      <c r="A2" s="21" t="s">
-        <v>108</v>
+    <row r="22" spans="1:11" ht="105">
+      <c r="A22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="43" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="43" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="43" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="43" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="43" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="43" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="43" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="43" customHeight="1" thickBot="1">
-      <c r="A11" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="43" customHeight="1" thickBot="1">
-      <c r="A12" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="43" customHeight="1">
-      <c r="A13" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="43" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="43" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="43" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="43" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="43" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>74</v>
+    <row r="23" spans="1:11" ht="105">
+      <c r="A23" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Test fix of GPAC
Test fix of GPAC
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -294,11 +294,6 @@
     <t>MP4Box -dash 20000 -frag 10000 -profile dashavc264:onDemand -rap counter_video_720.mp4 counter_audio.mp4 subtitles-10m-random-length.mp4 -out manifest-test-dash-20s-frag-10s-subs-rand-dashavc264</t>
   </si>
   <si>
-    <t>ERROR at generation:
-Assertion failed: (defaultDuration), function gf_media_isom_segment_file, file media_tools/dash_segmenter.c, line 1357.
-Abort trap: 6</t>
-  </si>
-  <si>
     <t>Plays, but displays between once and three times the subtitle on screen Don't see know the correlation for how many times it's displayed.</t>
   </si>
   <si>
@@ -459,13 +454,16 @@
   <si>
     <t>dashed 10s segments
 Duration Subs = 10s  A/V content &gt;= subs</t>
+  </si>
+  <si>
+    <t>Plays and then stop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -528,14 +526,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -556,7 +546,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,11 +576,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
@@ -601,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -621,21 +606,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,7 +743,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="214">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -886,8 +856,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -989,7 +966,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1012,46 +989,46 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="112" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="113" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="112" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="113" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="112" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="113" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="112" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="113" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="112" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,22 +1040,19 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="214">
+  <cellStyles count="221">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="113" builtinId="23"/>
+    <cellStyle name="Check Cell" xfId="112" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -1133,56 +1107,60 @@
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1238,59 +1216,62 @@
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="112" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1621,116 +1602,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="27"/>
+    <col min="1" max="1" width="10.83203125" style="26"/>
     <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
     <col min="3" max="12" width="28.5" style="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31" thickBot="1">
-      <c r="A1" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="17" customFormat="1" ht="35" customHeight="1" thickBot="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="35" customHeight="1" thickBot="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" ht="90">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="90">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>119</v>
+      <c r="B4" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>37</v>
@@ -1764,11 +1745,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="90">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>120</v>
+      <c r="B5" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>37</v>
@@ -1802,11 +1783,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="90">
-      <c r="A6" s="26">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>121</v>
+      <c r="B6" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
@@ -1840,11 +1821,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="90">
-      <c r="A7" s="26">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>122</v>
+      <c r="B7" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>41</v>
@@ -1878,11 +1859,11 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="90">
-      <c r="A8" s="26">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>123</v>
+      <c r="B8" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>41</v>
@@ -1916,11 +1897,11 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="90">
-      <c r="A9" s="26">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>124</v>
+      <c r="B9" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>59</v>
@@ -1954,11 +1935,11 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="105">
-      <c r="A10" s="26">
+      <c r="A10" s="25">
         <v>8</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>125</v>
+      <c r="B10" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>37</v>
@@ -1992,118 +1973,118 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="106" thickBot="1">
-      <c r="A11" s="26">
+      <c r="A11" s="25">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="17" customFormat="1" ht="35" customHeight="1" thickBot="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="19"/>
+    <row r="12" spans="1:12" s="16" customFormat="1" ht="35" customHeight="1" thickBot="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="105">
-      <c r="A13" s="26">
+      <c r="A13" s="25">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="15" t="s">
+      <c r="B13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="105">
-      <c r="A14" s="26">
+      <c r="A14" s="25">
         <v>11</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>128</v>
+      <c r="B14" s="23" t="s">
+        <v>127</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>66</v>
@@ -2121,26 +2102,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="120">
-      <c r="A15" s="26">
+    <row r="15" spans="1:12" ht="105">
+      <c r="A15" s="25">
         <v>12</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="5" t="s">
@@ -2160,26 +2141,26 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="105">
-      <c r="A16" s="26">
+      <c r="A16" s="25">
         <v>13</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>130</v>
+      <c r="B16" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>76</v>
@@ -2198,26 +2179,26 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="105">
-      <c r="A17" s="26">
+      <c r="A17" s="25">
         <v>14</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>131</v>
+      <c r="B17" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>81</v>
@@ -2235,27 +2216,27 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="121" thickBot="1">
-      <c r="A18" s="26">
+    <row r="18" spans="1:12" ht="106" thickBot="1">
+      <c r="A18" s="25">
         <v>15</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>91</v>
+      <c r="B18" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>86</v>
@@ -2273,120 +2254,120 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="17" customFormat="1" ht="35" customHeight="1" thickBot="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
+    <row r="19" spans="1:12" s="16" customFormat="1" ht="35" customHeight="1" thickBot="1">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="106" thickBot="1">
-      <c r="A20" s="26">
+      <c r="A20" s="25">
         <v>16</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>102</v>
-      </c>
       <c r="H20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="21" spans="1:12" s="17" customFormat="1" ht="35" customHeight="1" thickBot="1">
-      <c r="A21" s="28"/>
-      <c r="B21" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="21"/>
+    <row r="21" spans="1:12" s="16" customFormat="1" ht="35" customHeight="1" thickBot="1">
+      <c r="A21" s="27"/>
+      <c r="B21" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="22" spans="1:12" ht="105">
-      <c r="A22" s="26">
+      <c r="A22" s="25">
         <v>17</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>135</v>
+      <c r="B22" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="H22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="105">
-      <c r="A23" s="26">
+      <c r="A23" s="25">
         <v>18</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>134</v>
+      <c r="B23" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>37</v>
@@ -2401,26 +2382,26 @@
         <v>37</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="34" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">

</xml_diff>